<commit_message>
Add Authentication test casess
</commit_message>
<xml_diff>
--- a/test_case/Authentication/Registation/Tc_Reg_Security(nadira).xlsx
+++ b/test_case/Authentication/Registation/Tc_Reg_Security(nadira).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ai-quizwhiz.zluck.com-pnt-b24\test_case\Authentication\Registation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\my github project\ai-quizwhiz.zluck.com-pnt-b24\test_case\Authentication\Registation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1232,8 +1232,8 @@
   <dimension ref="A1:AA990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1764,15 +1764,27 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+    <row r="14" spans="1:27" ht="55.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1002</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -30062,7 +30074,7 @@
     <mergeCell ref="A1:H2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G13">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G14">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>